<commit_message>
:jigsaw: edit readme for reporting
</commit_message>
<xml_diff>
--- a/source/Data_compare.xlsx
+++ b/source/Data_compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670729FD-0C49-408C-83E0-E04E8B905B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7862E47A-1AF6-49BB-AEDC-E4175417412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -940,15 +940,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 10000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -960,6 +952,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$5:$B$15</c:f>
@@ -1053,15 +1103,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>50000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 50000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1073,6 +1115,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$5:$B$15</c:f>
@@ -1166,15 +1266,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$K$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>300000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 300000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1186,6 +1278,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$5:$B$15</c:f>
@@ -1276,8 +1426,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1573,15 +1724,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$C$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 10000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1593,6 +1736,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$22:$B$32</c:f>
@@ -1686,15 +1887,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$G$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>50000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 50000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1706,6 +1899,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$22:$B$32</c:f>
@@ -1799,15 +2050,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$K$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>300000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 300000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -1819,6 +2062,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$22:$B$32</c:f>
@@ -1909,8 +2210,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2196,15 +2498,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$C$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 10000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2216,6 +2510,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$39:$B$49</c:f>
@@ -2309,15 +2661,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$G$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>50000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 50000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2329,6 +2673,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$39:$B$49</c:f>
@@ -2422,15 +2824,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$K$37</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>300000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 300000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2442,6 +2836,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$39:$B$49</c:f>
@@ -2532,8 +2984,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2819,15 +3272,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$C$56</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 10000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2839,6 +3284,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$58:$B$68</c:f>
@@ -2932,15 +3435,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$G$56</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>50000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 50000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -2952,6 +3447,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$58:$B$68</c:f>
@@ -3045,15 +3598,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>RandomData!$K$56</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>300000</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Size 300000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -3065,6 +3610,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>RandomData!$B$58:$B$68</c:f>
@@ -3155,8 +3758,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -5977,8 +6581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V70" sqref="V70"/>
+    <sheetView tabSelected="1" topLeftCell="H45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X52" sqref="X52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>